<commit_message>
Add sample commands to .xlsx
</commit_message>
<xml_diff>
--- a/documentation/command_tests.xlsx
+++ b/documentation/command_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Adam\studia\2 sem\PROI\projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustaw\source\repos\graphic-file-converter\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37554543-CF37-4F38-833E-D496D3CC3DCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BD9F24-18D8-4066-AEBD-B2F0C42F99ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1635" yWindow="0" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit tests" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="226">
   <si>
     <t>komenda</t>
   </si>
@@ -698,6 +698,12 @@
   </si>
   <si>
     <t>../sample_bmps/font_out_negative.bmp'</t>
+  </si>
+  <si>
+    <t>graphic-file-converter.exe scan 1 45 '../font_bmps/bernardT.bmp' '../sample_bmps/found_letters/Bernard_font' -b</t>
+  </si>
+  <si>
+    <t>graphic-file-converter.exe scan 3 60 '../font_bmps/arial_f.bmp' '../sample_bmps/found_letters/ArialFont' -b</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1110,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1384,7 +1390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3334,9 +3340,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04D0369-A85D-4685-A6BC-7B7EC70BE0B1}">
-  <dimension ref="B1:B74"/>
+  <dimension ref="B1:B76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75:B76"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3713,6 +3721,16 @@
         <v>147</v>
       </c>
     </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>225</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>